<commit_message>
cart funtionality test cases started
</commit_message>
<xml_diff>
--- a/Test Documets/cart functionality test cases.xlsx
+++ b/Test Documets/cart functionality test cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>test case no</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>No product should be displayed in the cart</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
   <si>
     <t>SauceLabs backpack</t>
@@ -161,12 +164,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,70 +179,55 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -251,6 +239,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -259,10 +263,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -289,16 +293,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -314,13 +317,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -341,187 +337,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,22 +531,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,6 +563,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -579,17 +581,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -609,21 +620,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -635,148 +631,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1112,8 +1108,8 @@
   <sheetPr/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1144,7 +1140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="72" spans="1:5">
+    <row r="2" ht="72" spans="1:6">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1160,158 +1156,188 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" ht="115.2" spans="1:5">
+    <row r="3" ht="115.2" spans="1:6">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" ht="115.2" spans="1:5">
+    <row r="4" ht="115.2" spans="1:6">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" ht="115.2" spans="1:5">
+    <row r="5" ht="115.2" spans="1:6">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="6" ht="115.2" spans="1:5">
+    <row r="6" ht="115.2" spans="1:6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="7" ht="115.2" spans="1:5">
+    <row r="7" ht="115.2" spans="1:6">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="8" ht="115.2" spans="1:5">
+    <row r="8" ht="115.2" spans="1:6">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="9" ht="129.6" spans="1:5">
+    <row r="9" ht="129.6" spans="1:6">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="10" ht="144" spans="1:5">
+    <row r="10" ht="144" spans="1:6">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="11" ht="115.2" spans="1:5">
+    <row r="11" ht="115.2" spans="1:6">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>